<commit_message>
se subio las pr practicas
</commit_message>
<xml_diff>
--- a/2015-2016/clases/computacion_aplicada_2/clase_11/practicas/alex_naranjo.xlsx
+++ b/2015-2016/clases/computacion_aplicada_2/clase_11/practicas/alex_naranjo.xlsx
@@ -685,11 +685,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="121936384"/>
-        <c:axId val="121963648"/>
+        <c:axId val="87595520"/>
+        <c:axId val="67085440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="121936384"/>
+        <c:axId val="87595520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -698,7 +698,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121963648"/>
+        <c:crossAx val="67085440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -706,7 +706,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="121963648"/>
+        <c:axId val="67085440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -717,7 +717,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121936384"/>
+        <c:crossAx val="87595520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -844,11 +844,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="121937408"/>
-        <c:axId val="121965952"/>
+        <c:axId val="87596544"/>
+        <c:axId val="67087744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="121937408"/>
+        <c:axId val="87596544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -876,7 +876,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121965952"/>
+        <c:crossAx val="67087744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -884,7 +884,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="121965952"/>
+        <c:axId val="67087744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -913,7 +913,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121937408"/>
+        <c:crossAx val="87596544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1003,43 +1003,43 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>22</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>24</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>21</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1110,11 +1110,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="123809792"/>
-        <c:axId val="123065984"/>
+        <c:axId val="89925120"/>
+        <c:axId val="67089472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="123809792"/>
+        <c:axId val="89925120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1124,7 +1124,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123065984"/>
+        <c:crossAx val="67089472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1132,7 +1132,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="123065984"/>
+        <c:axId val="67089472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1143,7 +1143,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123809792"/>
+        <c:crossAx val="89925120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1316,7 +1316,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1394,7 +1394,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1433,7 +1433,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1472,7 +1472,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1511,7 +1511,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1550,7 +1550,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1589,7 +1589,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1667,7 +1667,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1706,7 +1706,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>21</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1745,7 +1745,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>21</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1784,7 +1784,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1799,11 +1799,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="122759680"/>
-        <c:axId val="121967680"/>
+        <c:axId val="87592960"/>
+        <c:axId val="67091200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="122759680"/>
+        <c:axId val="87592960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1812,7 +1812,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121967680"/>
+        <c:crossAx val="67091200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1820,7 +1820,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="121967680"/>
+        <c:axId val="67091200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1831,7 +1831,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122759680"/>
+        <c:crossAx val="87592960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2487,11 +2487,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="122760704"/>
-        <c:axId val="123060800"/>
+        <c:axId val="90157568"/>
+        <c:axId val="90065152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="122760704"/>
+        <c:axId val="90157568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2500,7 +2500,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123060800"/>
+        <c:crossAx val="90065152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2508,7 +2508,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="123060800"/>
+        <c:axId val="90065152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2519,7 +2519,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122760704"/>
+        <c:crossAx val="90157568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2717,11 +2717,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="122760192"/>
-        <c:axId val="123064256"/>
+        <c:axId val="89925632"/>
+        <c:axId val="90068608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="122760192"/>
+        <c:axId val="89925632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2731,7 +2731,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123064256"/>
+        <c:crossAx val="90068608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2739,7 +2739,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="123064256"/>
+        <c:axId val="90068608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2750,7 +2750,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122760192"/>
+        <c:crossAx val="89925632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3601,8 +3601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="23" zoomScaleNormal="23" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3705,7 +3705,7 @@
         <v>28</v>
       </c>
       <c r="D14" s="2">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E14" s="17">
         <v>1.6359999999999999</v>
@@ -3749,7 +3749,7 @@
         <v>30</v>
       </c>
       <c r="D16" s="2">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E16" s="17">
         <v>1.6659999999999999</v>
@@ -3771,7 +3771,7 @@
         <v>24</v>
       </c>
       <c r="D17" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" s="17">
         <v>1.681</v>
@@ -3793,7 +3793,7 @@
         <v>26</v>
       </c>
       <c r="D18" s="2">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E18" s="17">
         <v>1.696</v>
@@ -3815,7 +3815,7 @@
         <v>22</v>
       </c>
       <c r="D19" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E19" s="17">
         <v>1.7110000000000001</v>
@@ -3837,7 +3837,7 @@
         <v>13</v>
       </c>
       <c r="D20" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E20" s="17">
         <v>1.726</v>
@@ -3859,7 +3859,7 @@
         <v>12</v>
       </c>
       <c r="D21" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E21" s="17">
         <v>1.7410000000000001</v>
@@ -3903,7 +3903,7 @@
         <v>27</v>
       </c>
       <c r="D23" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E23" s="17">
         <v>1.77</v>
@@ -3925,7 +3925,7 @@
         <v>14</v>
       </c>
       <c r="D24" s="2">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E24" s="17">
         <v>1.78</v>
@@ -3947,7 +3947,7 @@
         <v>32</v>
       </c>
       <c r="D25" s="2">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E25" s="17">
         <v>1.8</v>
@@ -3969,7 +3969,7 @@
         <v>23</v>
       </c>
       <c r="D26" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E26" s="17">
         <v>1.82</v>
@@ -3987,8 +3987,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="C12:F26">
-    <sortCondition ref="E12"/>
+  <sortState ref="D12:D26">
+    <sortCondition ref="D12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>